<commit_message>
Remove 0/1 from BoolField. Fix #156
</commit_message>
<xml_diff>
--- a/tests/data/all-field-types.xlsx
+++ b/tests/data/all-field-types.xlsx
@@ -5,100 +5,106 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="976" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t>bool_column</t>
-  </si>
-  <si>
-    <t>integer_column</t>
-  </si>
-  <si>
-    <t>float_column</t>
-  </si>
-  <si>
-    <t>decimal_column</t>
-  </si>
-  <si>
-    <t>percent_column</t>
-  </si>
-  <si>
-    <t>date_column</t>
-  </si>
-  <si>
-    <t>datetime_column</t>
-  </si>
-  <si>
-    <t>unicode_column</t>
-  </si>
-  <si>
-    <t>null_column</t>
-  </si>
-  <si>
-    <t>Álvaro</t>
-  </si>
-  <si>
-    <t>àáãâä¹²³</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>éèẽêë</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>~~~~</t>
-  </si>
-  <si>
-    <t>nil</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>álvaro</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>n/a</t>
+    <t xml:space="preserve">bool_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimal_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unicode_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Álvaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">àáãâä¹²³</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">éèẽêë</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~~~~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">álvaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.00%"/>
-    <numFmt numFmtId="166" formatCode="MMM\ D&quot;, &quot;YYYY"/>
-    <numFmt numFmtId="167" formatCode="YYYY\-MM\-DD\ HH:MM:SS"/>
-    <numFmt numFmtId="168" formatCode="@"/>
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="167" formatCode="MMM\ D&quot;, &quot;YYYY"/>
+    <numFmt numFmtId="168" formatCode="YYYY\-MM\-DD\ HH:MM:SS"/>
+    <numFmt numFmtId="169" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -165,7 +171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,7 +188,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -206,15 +216,15 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.1020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.4489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -247,7 +257,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -259,13 +269,13 @@
       <c r="D2" s="0" t="n">
         <v>3.141592</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <v>42005</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="G2" s="4" t="n">
         <v>42234.6319444444</v>
       </c>
       <c r="H2" s="0" t="s">
@@ -273,7 +283,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -285,13 +295,13 @@
       <c r="D3" s="0" t="n">
         <v>1.234</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>0.1169</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="3" t="n">
         <v>36194</v>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="4" t="n">
         <v>36194.0007175926</v>
       </c>
       <c r="H3" s="0" t="s">
@@ -302,7 +312,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -314,13 +324,13 @@
       <c r="D4" s="0" t="n">
         <v>4.56</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>0.12</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="3" t="n">
         <v>54790</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="4" t="n">
         <v>54790.9899421296</v>
       </c>
       <c r="H4" s="0" t="s">
@@ -331,7 +341,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -343,13 +353,13 @@
       <c r="D5" s="0" t="n">
         <v>7.89</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>0.1364</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="3" t="n">
         <v>42234</v>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="G5" s="4" t="n">
         <v>42234.9316319445</v>
       </c>
       <c r="H5" s="0" t="s">
@@ -372,13 +382,13 @@
       <c r="D6" s="0" t="n">
         <v>9.87</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>0.1314</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="3" t="n">
         <v>42067</v>
       </c>
-      <c r="G6" s="3" t="n">
+      <c r="G6" s="4" t="n">
         <v>42067.6666782407</v>
       </c>
       <c r="H6" s="0" t="s">
@@ -401,13 +411,13 @@
       <c r="D7" s="0" t="n">
         <v>1.2345</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>0.02</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="3" t="n">
         <v>42130</v>
       </c>
-      <c r="G7" s="3" t="n">
+      <c r="G7" s="4" t="n">
         <v>42130.5007175926</v>
       </c>
       <c r="H7" s="0" t="s">

</xml_diff>

<commit_message>
Change SQLite, XLS and XLSX test data
</commit_message>
<xml_diff>
--- a/tests/data/all-field-types.xlsx
+++ b/tests/data/all-field-types.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">bool_column</t>
   </si>
@@ -46,49 +46,46 @@
     <t xml:space="preserve">unicode_column</t>
   </si>
   <si>
-    <t xml:space="preserve">null_column</t>
-  </si>
-  <si>
     <t xml:space="preserve">Álvaro</t>
   </si>
   <si>
     <t xml:space="preserve">àáãâä¹²³</t>
   </si>
   <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">éèẽêë</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~~~~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">álvaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
     <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">éèẽêë</t>
-  </si>
-  <si>
     <t xml:space="preserve">null</t>
   </si>
   <si>
-    <t xml:space="preserve">false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~~~~</t>
-  </si>
-  <si>
     <t xml:space="preserve">nil</t>
   </si>
   <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">álvaro</t>
-  </si>
-  <si>
     <t xml:space="preserve">none</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
   </si>
   <si>
     <t xml:space="preserve">n/a</t>
@@ -213,21 +210,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -252,12 +247,10 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="b">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -279,11 +272,12 @@
         <v>42234.6319444444</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="b">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -305,15 +299,12 @@
         <v>36194.0007175926</v>
       </c>
       <c r="H3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3</v>
@@ -334,15 +325,12 @@
         <v>54790.9899421296</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
@@ -363,15 +351,12 @@
         <v>42234.9316319445</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>5</v>
@@ -392,15 +377,12 @@
         <v>42067.6666782407</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>6</v>
@@ -421,10 +403,27 @@
         <v>42130.5007175926</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="0" t="s">
-        <v>23</v>
+      <c r="G8" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extract only data from XLSX (+ fix warning)
</commit_message>
<xml_diff>
--- a/tests/data/all-field-types.xlsx
+++ b/tests/data/all-field-types.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -95,13 +95,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="MMM\ D&quot;, &quot;YYYY"/>
     <numFmt numFmtId="168" formatCode="YYYY\-MM\-DD\ HH:MM:SS"/>
     <numFmt numFmtId="169" formatCode="@"/>
+    <numFmt numFmtId="170" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -168,7 +169,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,6 +191,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -210,16 +215,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -249,8 +256,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="A2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -276,8 +282,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="A3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -407,6 +412,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6"/>
       <c r="B8" s="0" t="s">
         <v>18</v>
       </c>
@@ -426,10 +432,11 @@
         <v>19</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.3" right="0.3" top="0.609722222222222" bottom="0.370138888888889" header="0.1" footer="0.1"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;P</oddHeader>
     <oddFooter>&amp;C&amp;F</oddFooter>

</xml_diff>

<commit_message>
Enhance start_row/column behaviour on XLS/XLSX
</commit_message>
<xml_diff>
--- a/tests/data/all-field-types.xlsx
+++ b/tests/data/all-field-types.xlsx
@@ -95,14 +95,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="MMM\ D&quot;, &quot;YYYY"/>
     <numFmt numFmtId="168" formatCode="YYYY\-MM\-DD\ HH:MM:SS"/>
     <numFmt numFmtId="169" formatCode="@"/>
-    <numFmt numFmtId="170" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -169,7 +168,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -191,21 +190,17 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -215,10 +210,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="C1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -226,213 +221,219 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="b">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="E5" s="0" t="n">
         <v>3.141592</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="F5" s="0" t="n">
         <v>3.141592</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="G5" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="H5" s="3" t="n">
         <v>42005</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="I5" s="4" t="n">
         <v>42234.6319444444</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="J5" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="b">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="1" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="D6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="E6" s="0" t="n">
         <v>1.234</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="F6" s="0" t="n">
         <v>1.234</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="G6" s="2" t="n">
         <v>0.1169</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="H6" s="3" t="n">
         <v>36194</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="I6" s="4" t="n">
         <v>36194.0007175926</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="J6" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="D7" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="E7" s="0" t="n">
         <v>4.56</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="F7" s="0" t="n">
         <v>4.56</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="G7" s="2" t="n">
         <v>0.12</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="H7" s="3" t="n">
         <v>54790</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="I7" s="4" t="n">
         <v>54790.9899421296</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="J7" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="D8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <v>7.89</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="F8" s="0" t="n">
         <v>7.89</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="G8" s="2" t="n">
         <v>0.1364</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="H8" s="3" t="n">
         <v>42234</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="I8" s="4" t="n">
         <v>42234.9316319445</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="J8" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="D9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="E9" s="0" t="n">
         <v>9.87</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="F9" s="0" t="n">
         <v>9.87</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="G9" s="2" t="n">
         <v>0.1314</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="H9" s="3" t="n">
         <v>42067</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="I9" s="4" t="n">
         <v>42067.6666782407</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="J9" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="D10" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="E10" s="0" t="n">
         <v>1.2345</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="F10" s="0" t="n">
         <v>1.2345</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="G10" s="2" t="n">
         <v>0.02</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="H10" s="3" t="n">
         <v>42130</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="I10" s="4" t="n">
         <v>42130.5007175926</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="J10" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="0" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="1"/>
+      <c r="D11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="E11" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="F11" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="G11" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="H11" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="I11" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.3" right="0.3" top="0.609722222222222" bottom="0.370138888888889" header="0.1" footer="0.1"/>

</xml_diff>